<commit_message>
Add files via upload
</commit_message>
<xml_diff>
--- a/SIpON v3 alfa/kn.xlsx
+++ b/SIpON v3 alfa/kn.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Пользователь\Documents\py\SIpON v3 alfa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4AE3C5-633C-438F-8178-F425D445D31D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0E46AC-00EF-407F-9628-D22F8AC33071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KN" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet KN" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet KN" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="56">
   <si>
     <t>KN</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Актуально</t>
   </si>
   <si>
-    <t>56.7</t>
-  </si>
-  <si>
     <t>кв.м</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
     <t>11.12.2020</t>
   </si>
   <si>
-    <t>1500</t>
-  </si>
-  <si>
     <t>обл. Волгоградская, р-н Быковский, с. Кислово,, ул. Песчаная, дом 4</t>
   </si>
   <si>
@@ -137,9 +131,6 @@
     <t>12.12.2020</t>
   </si>
   <si>
-    <t>39.6</t>
-  </si>
-  <si>
     <t>Волгоградская область, р-н. Быковский, с. Кислово, ул. Песчаная, д. 4</t>
   </si>
   <si>
@@ -152,9 +143,6 @@
     <t>29.12.2020</t>
   </si>
   <si>
-    <t>1512</t>
-  </si>
-  <si>
     <t>обл. Волгоградская, р-н Быковский, п. Приморск, ул. Советская, дом 23</t>
   </si>
   <si>
@@ -164,9 +152,6 @@
     <t>26.03.2021</t>
   </si>
   <si>
-    <t>51.3</t>
-  </si>
-  <si>
     <t>Волгоградская область, р-н. Быковский, с. Приморск, ул. Советская, д. 23</t>
   </si>
   <si>
@@ -176,9 +161,6 @@
     <t>Помещение</t>
   </si>
   <si>
-    <t>58.1</t>
-  </si>
-  <si>
     <t>Волгоградская область, р-н. Быковский, рп. Быково, ул. Куйбышева, д. 14, кв. 8</t>
   </si>
   <si>
@@ -188,18 +170,12 @@
     <t>19.12.2020</t>
   </si>
   <si>
-    <t>42.5</t>
-  </si>
-  <si>
     <t>Волгоградская область, г. Волжский, пр-кт. Ленина, д. 186, кв. 23</t>
   </si>
   <si>
     <t>18.05.2015</t>
   </si>
   <si>
-    <t>21.5</t>
-  </si>
-  <si>
     <t>Волгоградская область, г. Волжский, ул. Машиностроителей, д. 19, к. 138</t>
   </si>
   <si>
@@ -207,9 +183,6 @@
   </si>
   <si>
     <t>22.12.2020</t>
-  </si>
-  <si>
-    <t>74</t>
   </si>
   <si>
     <t>Волгоградская область, г. Волжский, ул. Пионерская, д. 19, кв. 144</t>
@@ -1017,7 +990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1093,10 +1066,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1142,20 +1115,20 @@
       <c r="D2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2">
+        <v>56.7</v>
+      </c>
+      <c r="F2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>25</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>26</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>27</v>
-      </c>
-      <c r="I2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1163,13 +1136,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
         <v>29</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1177,28 +1150,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4">
+        <v>1500</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" t="s">
         <v>33</v>
       </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>34</v>
-      </c>
-      <c r="H4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1206,7 +1179,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
@@ -1214,20 +1187,20 @@
       <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" t="s">
-        <v>38</v>
+      <c r="E5">
+        <v>39.6</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1235,13 +1208,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
         <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1249,28 +1222,28 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
         <v>23</v>
       </c>
-      <c r="E7" t="s">
-        <v>43</v>
+      <c r="E7">
+        <v>1512</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1278,7 +1251,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
@@ -1286,20 +1259,20 @@
       <c r="D8" t="s">
         <v>23</v>
       </c>
-      <c r="E8" t="s">
-        <v>47</v>
+      <c r="E8">
+        <v>51.3</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1307,28 +1280,28 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D9" t="s">
         <v>23</v>
       </c>
-      <c r="E9" t="s">
-        <v>51</v>
+      <c r="E9">
+        <v>58.1</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1336,28 +1309,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D10" t="s">
         <v>23</v>
       </c>
-      <c r="E10" t="s">
-        <v>55</v>
+      <c r="E10">
+        <v>42.5</v>
       </c>
       <c r="F10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G10" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I10" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1365,28 +1338,28 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
         <v>23</v>
       </c>
-      <c r="E11" t="s">
-        <v>58</v>
+      <c r="E11">
+        <v>21.5</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G11" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I11" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1394,28 +1367,28 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D12" t="s">
         <v>23</v>
       </c>
-      <c r="E12" t="s">
-        <v>62</v>
+      <c r="E12">
+        <v>74</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="H12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I12" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>